<commit_message>
start for multimedia handling, continue to refine this and make the new file management system
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toby Tatsuya\TimeLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B18F7509-7617-43CE-9C0C-A283EF65C21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFACA2B-A2A1-40D6-97C8-984A2A1DEAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="12160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Year</t>
   </si>
@@ -61,49 +61,84 @@
     <t>Background_url</t>
   </si>
   <si>
-    <t>TimeSpan Title</t>
-  </si>
-  <si>
-    <t>Example Text for this TimeSpan</t>
-  </si>
-  <si>
     <t>download.jpeg</t>
   </si>
   <si>
-    <t>Media Credit Text</t>
-  </si>
-  <si>
     <t>Media Caption</t>
   </si>
   <si>
     <t>#3333f3</t>
   </si>
   <si>
-    <t>Single day event</t>
-  </si>
-  <si>
-    <t>Here is the text for that</t>
-  </si>
-  <si>
-    <t>Media Credit Text 2</t>
-  </si>
-  <si>
-    <t>Image Caption 2</t>
-  </si>
-  <si>
-    <t>#222222</t>
-  </si>
-  <si>
-    <t>Second Timespan</t>
-  </si>
-  <si>
     <t>Text for this</t>
+  </si>
+  <si>
+    <t>untitled-3.mp3</t>
+  </si>
+  <si>
+    <t>Lauren Cockerill</t>
+  </si>
+  <si>
+    <t>Norwegian Wood - live in the Vern</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>KANGA.mp4</t>
+  </si>
+  <si>
+    <t>THIS IS A VIDEO OF A KANGAROO</t>
+  </si>
+  <si>
+    <t>This has no image</t>
+  </si>
+  <si>
+    <t>Will this handle No image ok?</t>
+  </si>
+  <si>
+    <t>Hour</t>
+  </si>
+  <si>
+    <t>Minute</t>
+  </si>
+  <si>
+    <t>End_Hour</t>
+  </si>
+  <si>
+    <t>End_Minute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example </t>
+  </si>
+  <si>
+    <t>Example 2</t>
+  </si>
+  <si>
+    <t>Here is more text for this event</t>
+  </si>
+  <si>
+    <t>Media Credit</t>
+  </si>
+  <si>
+    <t>The following stories contain memorials to the children who have been part of our life and are now remembered in words of love. Just three things remain, faith, hope and love. The greatest of these is love. Corinthians, Ch.13; V.13.</t>
+  </si>
+  <si>
+    <t>Official opening of the Centre by Lady Stoddart. Established to offer services to anyone affected by the death of a child.
+&lt;br&gt;&lt;br&gt;
+When a child dies...&lt;br&gt;
+The death of a child is one of the most devastating events that can happen to any family.
+&lt;br&gt;&lt;br&gt;
+The pain may be greater than any other have felt. However, even at its most distressing the pain of grief is a natural reaction at that time.
+&lt;br&gt;&lt;br&gt;
+At times the emotional and physical symptoms can be so overwhelming that they make everyday living very difficult.&lt;br&gt;&lt;br&gt;
+Surviving the pain of grief may seem impossible for a long time. Family, friends and others can be an important source of support but sometimes people need extra help.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -240,7 +275,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -422,18 +457,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -549,31 +578,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -622,14 +637,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -984,161 +997,213 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="8.7265625" style="4"/>
-    <col min="5" max="5" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.26953125" customWidth="1"/>
-    <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="8.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="32.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="67.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="24.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="2" spans="1:17" ht="234" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2010</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="1">
         <v>4</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C3" s="1">
         <v>20</v>
       </c>
-      <c r="D2">
+      <c r="D3" s="1">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1">
+        <v>35</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>2010</v>
       </c>
-      <c r="E2">
+      <c r="B4" s="1">
         <v>4</v>
       </c>
-      <c r="F2" s="4">
+      <c r="C4" s="1">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1">
+        <v>36</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1">
+        <v>37</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1">
+        <v>38</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" t="s">
+      <c r="L6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2010</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>2010</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4">
-        <v>22</v>
-      </c>
-      <c r="D4">
-        <v>2010</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4" s="4">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
working auto html, next styles, and try to implement auto scrolling when idle
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toby Tatsuya\TimeLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFACA2B-A2A1-40D6-97C8-984A2A1DEAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF890A8-59E9-4079-A6A2-6DCF36D0D7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="12160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Year</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Background_url</t>
   </si>
   <si>
-    <t>download.jpeg</t>
-  </si>
-  <si>
     <t>Media Caption</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t>Text for this</t>
   </si>
   <si>
-    <t>untitled-3.mp3</t>
-  </si>
-  <si>
     <t>Lauren Cockerill</t>
   </si>
   <si>
@@ -83,9 +77,6 @@
   </si>
   <si>
     <t>Third</t>
-  </si>
-  <si>
-    <t>KANGA.mp4</t>
   </si>
   <si>
     <t>THIS IS A VIDEO OF A KANGAROO</t>
@@ -133,6 +124,42 @@
 &lt;br&gt;&lt;br&gt;
 At times the emotional and physical symptoms can be so overwhelming that they make everyday living very difficult.&lt;br&gt;&lt;br&gt;
 Surviving the pain of grief may seem impossible for a long time. Family, friends and others can be an important source of support but sometimes people need extra help.</t>
+  </si>
+  <si>
+    <t>exampleImg</t>
+  </si>
+  <si>
+    <t>exampleAud</t>
+  </si>
+  <si>
+    <t>exampleVid</t>
+  </si>
+  <si>
+    <t>exampleMulti</t>
+  </si>
+  <si>
+    <t>Multi test</t>
+  </si>
+  <si>
+    <t>Test for multi</t>
+  </si>
+  <si>
+    <t>new image set</t>
+  </si>
+  <si>
+    <t>demo</t>
+  </si>
+  <si>
+    <t>demo2</t>
+  </si>
+  <si>
+    <t>Here will be 5 images</t>
+  </si>
+  <si>
+    <t>exampleimg</t>
+  </si>
+  <si>
+    <t>out of order</t>
   </si>
 </sst>
 </file>
@@ -998,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,8 +1044,7 @@
     <col min="13" max="13" width="17.42578125" style="1" customWidth="1"/>
     <col min="14" max="14" width="24.7109375" style="1" customWidth="1"/>
     <col min="15" max="15" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="17.42578125" style="1" customWidth="1"/>
     <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1033,10 +1059,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -1048,10 +1074,10 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>6</v>
@@ -1077,10 +1103,10 @@
     </row>
     <row r="2" spans="1:17" ht="234" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K2" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -1097,25 +1123,16 @@
         <v>12</v>
       </c>
       <c r="E3" s="1">
+        <v>30</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -1132,22 +1149,25 @@
         <v>12</v>
       </c>
       <c r="E4" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1164,16 +1184,25 @@
         <v>12</v>
       </c>
       <c r="E5" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -1190,16 +1219,96 @@
         <v>12</v>
       </c>
       <c r="E6" s="1">
+        <v>37</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1">
         <v>38</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>13</v>
+      <c r="K7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>21</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>22</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>19</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added controls for navbar size
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toby Tatsuya\TimeLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B4C5EB-4749-4688-AE37-272EAE05D283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467B8637-5C90-4C1A-92D2-EC9F4BBF3F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -682,9 +682,9 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1043,33 +1043,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
-    <col min="2" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="8.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="32.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="67.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="17.42578125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="24.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="21.140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1796875" style="1" customWidth="1"/>
+    <col min="2" max="4" width="9.1796875" style="1"/>
+    <col min="5" max="5" width="8.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.1796875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.81640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="32.7265625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="67.453125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.453125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="24.7265625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="14.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.453125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="21.1796875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="9" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:22" s="9" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1127,7 +1127,7 @@
       <c r="U1" s="6"/>
       <c r="V1" s="6"/>
     </row>
-    <row r="2" spans="1:22" s="3" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" s="3" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -1152,7 +1152,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="300" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2010</v>
       </c>
@@ -1189,6 +1189,26 @@
       <c r="Q3" s="1" t="s">
         <v>19</v>
       </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>